<commit_message>
16 Agustus 2023 Upload
</commit_message>
<xml_diff>
--- a/RealCode/RSF/BIMASAKTI_11/1.00/PROGRAM/BS Program/SOURCE/API/GS/BIMASAKTI_GS_API/Template/Cash Flow Plan.xlsx
+++ b/RealCode/RSF/BIMASAKTI_11/1.00/PROGRAM/BS Program/SOURCE/API/GS/BIMASAKTI_GS_API/Template/Cash Flow Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Work\BIMASAKTI 11\Program Specs\GS\Upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DB5A36-76E2-438E-B1D3-78C07AFA75C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B93FFBE-6025-422C-B6F5-B49AF130D188}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940" xr2:uid="{1FF24E20-BBC6-43C0-86AE-C6375945D9D5}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>No.</t>
   </si>
@@ -85,9 +85,6 @@
     <t>PeriodNo</t>
   </si>
   <si>
-    <t>Amount</t>
-  </si>
-  <si>
     <t>CashFlow Plan</t>
   </si>
   <si>
@@ -104,6 +101,18 @@
   </si>
   <si>
     <t>01</t>
+  </si>
+  <si>
+    <t>LocalAmount</t>
+  </si>
+  <si>
+    <t>BaseAmount</t>
+  </si>
+  <si>
+    <t>Local Amount</t>
+  </si>
+  <si>
+    <t>Base Amount</t>
   </si>
 </sst>
 </file>
@@ -495,36 +504,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D1A87FA-2433-46F8-AC5D-D5A065704D53}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -536,10 +550,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A8A5E21-C618-4BCA-95F1-7AD3EE4B7A52}">
-  <dimension ref="A2:M13"/>
+  <dimension ref="A2:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,7 +586,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -618,7 +632,7 @@
         <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
         <v>15</v>
@@ -630,7 +644,7 @@
         <v>2</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -638,19 +652,19 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" t="s">
         <v>23</v>
-      </c>
-      <c r="G8" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -658,27 +672,47 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>9</v>
       </c>
-      <c r="E9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
-        <v>12</v>
+      <c r="E10" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>